<commit_message>
Organize characteristics and add word IDs
</commit_message>
<xml_diff>
--- a/materials/readAloud-ldt/stimuli/ldt/ldt-stimuli_characteristics.xlsx
+++ b/materials/readAloud-ldt/stimuli/ldt/ldt-stimuli_characteristics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessraissouni/github/readAloud-valence-dataset/materials/readAloud-ldt/stimuli/ldt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81F62BD-5CBF-CA44-9B6D-DD060A847D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9843E43E-1D1F-4C42-8594-7040B77F1875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24540" windowHeight="15240" xr2:uid="{9AD4381F-A480-9043-B552-F4C6CA905AB8}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>dominance-WAR</t>
   </si>
   <si>
-    <t>ELP (Emotional_Valence)</t>
-  </si>
-  <si>
     <t>ELP (Emotional_Arousal)</t>
   </si>
   <si>
@@ -565,6 +562,9 @@
   </si>
   <si>
     <t>Excel =len()</t>
+  </si>
+  <si>
+    <t>Warriner et al. (2013)</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:AB115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,19 +984,19 @@
   <sheetData>
     <row r="1" spans="1:28" s="8" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>22</v>
+        <v>179</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>12</v>
@@ -1005,26 +1005,26 @@
         <v>15</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="O1" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>10</v>
@@ -1033,37 +1033,37 @@
         <v>11</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="U1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="W1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="AA1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1071,7 +1071,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -1080,7 +1080,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -1089,16 +1089,16 @@
         <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>18</v>
@@ -1110,7 +1110,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>7</v>
@@ -1119,7 +1119,7 @@
         <v>9</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>2</v>
@@ -1128,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>3</v>
@@ -1137,27 +1137,27 @@
         <v>4</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Z2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="1">
         <v>2.0499999999999998</v>
@@ -1181,7 +1181,7 @@
         <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L3" s="1">
         <v>6.26</v>
@@ -1232,18 +1232,18 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1">
         <v>5.64</v>
@@ -1264,10 +1264,10 @@
         <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M4" s="1">
         <v>4.1900000000000004</v>
@@ -1294,7 +1294,7 @@
         <v>2.46</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V4" s="2">
         <v>2330</v>
@@ -1315,18 +1315,18 @@
         <v>1</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="1">
         <v>6.04</v>
@@ -1347,10 +1347,10 @@
         <v>6</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M5" s="1">
         <v>3.67</v>
@@ -1377,7 +1377,7 @@
         <v>3.04</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V5" s="2">
         <v>5554.6</v>
@@ -1398,15 +1398,15 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" s="1">
         <v>8.39</v>
@@ -1430,7 +1430,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L6" s="1">
         <v>6.21</v>
@@ -1460,7 +1460,7 @@
         <v>2.2200000000000002</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V6" s="2">
         <v>3557.75</v>
@@ -1481,18 +1481,18 @@
         <v>1</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D7" s="1">
         <v>5.17</v>
@@ -1513,10 +1513,10 @@
         <v>5</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M7" s="1">
         <v>2.5</v>
@@ -1564,15 +1564,15 @@
         <v>1</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
@@ -1596,7 +1596,7 @@
         <v>7</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L8" s="1">
         <v>5.18</v>
@@ -1626,7 +1626,7 @@
         <v>2.86</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V8" s="2">
         <v>1814.1669999999999</v>
@@ -1647,24 +1647,24 @@
         <v>1</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F9" s="1">
         <v>7.9710000000000001</v>
@@ -1679,16 +1679,16 @@
         <v>5</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O9" s="1">
         <v>5.2089999999999996</v>
@@ -1730,15 +1730,15 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" s="1">
         <v>2.77</v>
@@ -1762,7 +1762,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L10" s="1">
         <v>4.93</v>
@@ -1813,18 +1813,18 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D11" s="1">
         <v>5.3</v>
@@ -1845,10 +1845,10 @@
         <v>4</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M11" s="1">
         <v>3.95</v>
@@ -1896,18 +1896,18 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D12" s="1">
         <v>4.4400000000000004</v>
@@ -1928,10 +1928,10 @@
         <v>6</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M12" s="1">
         <v>4.2</v>
@@ -1979,15 +1979,15 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C13" s="1">
         <v>7.11</v>
@@ -2011,7 +2011,7 @@
         <v>7</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L13" s="1">
         <v>4.71</v>
@@ -2062,18 +2062,18 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" s="1">
         <v>3.9</v>
@@ -2094,10 +2094,10 @@
         <v>6</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M14" s="1">
         <v>4.67</v>
@@ -2124,7 +2124,7 @@
         <v>4.78</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V14" s="2">
         <v>4639.3999999999996</v>
@@ -2145,18 +2145,18 @@
         <v>1</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" s="1">
         <v>5.48</v>
@@ -2177,10 +2177,10 @@
         <v>8</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M15" s="1">
         <v>3.71</v>
@@ -2228,15 +2228,15 @@
         <v>1</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C16" s="1">
         <v>5.33</v>
@@ -2260,7 +2260,7 @@
         <v>6</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L16" s="1">
         <v>3.17</v>
@@ -2311,15 +2311,15 @@
         <v>1</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" s="1">
         <v>1.5</v>
@@ -2343,7 +2343,7 @@
         <v>6</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L17" s="1">
         <v>6.42</v>
@@ -2394,15 +2394,15 @@
         <v>1</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="1">
         <v>8.3699999999999992</v>
@@ -2426,7 +2426,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L18" s="1">
         <v>7.37</v>
@@ -2477,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
@@ -2485,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D19" s="1">
         <v>5.14</v>
@@ -2509,10 +2509,10 @@
         <v>5</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M19" s="1">
         <v>3.48</v>
@@ -2560,15 +2560,15 @@
         <v>1</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" s="1">
         <v>8.44</v>
@@ -2592,7 +2592,7 @@
         <v>8</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L20" s="1">
         <v>5.85</v>
@@ -2622,7 +2622,7 @@
         <v>3.82</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V20" s="2">
         <v>3388.2860000000001</v>
@@ -2643,18 +2643,18 @@
         <v>1</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D21" s="1">
         <v>4.82</v>
@@ -2675,10 +2675,10 @@
         <v>7</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M21" s="1">
         <v>4.3499999999999996</v>
@@ -2726,15 +2726,15 @@
         <v>1</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="1">
         <v>7.3</v>
@@ -2758,7 +2758,7 @@
         <v>6</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L22" s="1">
         <v>5.97</v>
@@ -2809,18 +2809,18 @@
         <v>0.96299999999999997</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D23" s="1">
         <v>6.05</v>
@@ -2841,10 +2841,10 @@
         <v>7</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M23" s="1">
         <v>3.6</v>
@@ -2892,15 +2892,15 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C24" s="1">
         <v>3.46</v>
@@ -2924,7 +2924,7 @@
         <v>9</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L24" s="1">
         <v>6.07</v>
@@ -2954,7 +2954,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V24" s="2">
         <v>4133.75</v>
@@ -2975,15 +2975,15 @@
         <v>1</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C25" s="1">
         <v>2.1800000000000002</v>
@@ -3007,7 +3007,7 @@
         <v>6</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L25" s="1">
         <v>4.74</v>
@@ -3058,15 +3058,15 @@
         <v>1</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C26" s="1">
         <v>2.89</v>
@@ -3090,7 +3090,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L26" s="1">
         <v>5.41</v>
@@ -3141,15 +3141,15 @@
         <v>1</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C27" s="1">
         <v>5.9</v>
@@ -3173,7 +3173,7 @@
         <v>7</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L27" s="1">
         <v>4.9000000000000004</v>
@@ -3203,7 +3203,7 @@
         <v>2.04</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V27" s="2">
         <v>2800</v>
@@ -3224,15 +3224,15 @@
         <v>1</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C28" s="1">
         <v>2.2200000000000002</v>
@@ -3256,7 +3256,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L28" s="1">
         <v>5.68</v>
@@ -3307,18 +3307,18 @@
         <v>0.92600000000000005</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D29" s="1">
         <v>5.3</v>
@@ -3339,10 +3339,10 @@
         <v>6</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M29" s="1">
         <v>4.05</v>
@@ -3369,7 +3369,7 @@
         <v>4.07</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V29" s="2">
         <v>1972.6</v>
@@ -3390,15 +3390,15 @@
         <v>1</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C30" s="1">
         <v>2.64</v>
@@ -3422,7 +3422,7 @@
         <v>7</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L30" s="1">
         <v>6.83</v>
@@ -3473,15 +3473,15 @@
         <v>1</v>
       </c>
       <c r="AB30" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C31" s="1">
         <v>7.92</v>
@@ -3505,7 +3505,7 @@
         <v>7</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L31" s="1">
         <v>5.53</v>
@@ -3556,18 +3556,18 @@
         <v>1</v>
       </c>
       <c r="AB31" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D32" s="1">
         <v>5.24</v>
@@ -3588,10 +3588,10 @@
         <v>9</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M32" s="1">
         <v>3.73</v>
@@ -3618,7 +3618,7 @@
         <v>2.5</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V32" s="2">
         <v>4478.25</v>
@@ -3639,15 +3639,15 @@
         <v>1</v>
       </c>
       <c r="AB32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C33" s="1">
         <v>2.0299999999999998</v>
@@ -3671,7 +3671,7 @@
         <v>7</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L33" s="1">
         <v>5.32</v>
@@ -3722,18 +3722,18 @@
         <v>1</v>
       </c>
       <c r="AB33" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1">
         <v>2.52</v>
@@ -3754,10 +3754,10 @@
         <v>7</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M34" s="1">
         <v>4.55</v>
@@ -3805,15 +3805,15 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="AB34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C35" s="1">
         <v>5.3</v>
@@ -3837,7 +3837,7 @@
         <v>5</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L35" s="1">
         <v>3.98</v>
@@ -3888,15 +3888,15 @@
         <v>1</v>
       </c>
       <c r="AB35" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C36" s="1">
         <v>6.17</v>
@@ -3920,7 +3920,7 @@
         <v>4</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L36" s="1">
         <v>5.07</v>
@@ -3971,15 +3971,15 @@
         <v>1</v>
       </c>
       <c r="AB36" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" s="1">
         <v>6.69</v>
@@ -4003,7 +4003,7 @@
         <v>9</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L37" s="1">
         <v>5.74</v>
@@ -4054,15 +4054,15 @@
         <v>1</v>
       </c>
       <c r="AB37" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="1">
         <v>3.41</v>
@@ -4086,7 +4086,7 @@
         <v>9</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L38" s="1">
         <v>6.32</v>
@@ -4137,18 +4137,18 @@
         <v>1</v>
       </c>
       <c r="AB38" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D39" s="1">
         <v>2.2200000000000002</v>
@@ -4169,10 +4169,10 @@
         <v>5</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M39" s="1">
         <v>5.3</v>
@@ -4220,18 +4220,18 @@
         <v>1</v>
       </c>
       <c r="AB39" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D40" s="1">
         <v>3.36</v>
@@ -4252,10 +4252,10 @@
         <v>5</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M40" s="1">
         <v>4.43</v>
@@ -4303,15 +4303,15 @@
         <v>1</v>
       </c>
       <c r="AB40" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="1">
         <v>1.7</v>
@@ -4335,7 +4335,7 @@
         <v>7</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L41" s="1">
         <v>4.95</v>
@@ -4386,15 +4386,15 @@
         <v>1</v>
       </c>
       <c r="AB41" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C42" s="1">
         <v>3.04</v>
@@ -4418,7 +4418,7 @@
         <v>7</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L42" s="1">
         <v>3.46</v>
@@ -4469,18 +4469,18 @@
         <v>1</v>
       </c>
       <c r="AB42" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D43" s="1">
         <v>4.8099999999999996</v>
@@ -4501,10 +4501,10 @@
         <v>7</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M43" s="1">
         <v>5.6</v>
@@ -4552,15 +4552,15 @@
         <v>1</v>
       </c>
       <c r="AB43" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C44" s="1">
         <v>1.88</v>
@@ -4584,7 +4584,7 @@
         <v>5</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L44" s="1">
         <v>3.83</v>
@@ -4635,15 +4635,15 @@
         <v>1</v>
       </c>
       <c r="AB44" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C45" s="1">
         <v>7.55</v>
@@ -4667,7 +4667,7 @@
         <v>5</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L45" s="1">
         <v>6.02</v>
@@ -4718,18 +4718,18 @@
         <v>1</v>
       </c>
       <c r="AB45" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D46" s="1">
         <v>5.28</v>
@@ -4750,10 +4750,10 @@
         <v>6</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M46" s="1">
         <v>2.7</v>
@@ -4801,18 +4801,18 @@
         <v>1</v>
       </c>
       <c r="AB46" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D47" s="1">
         <v>5.18</v>
@@ -4833,10 +4833,10 @@
         <v>5</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M47" s="1">
         <v>4.75</v>
@@ -4884,15 +4884,15 @@
         <v>1</v>
       </c>
       <c r="AB47" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C48" s="1">
         <v>8.19</v>
@@ -4916,7 +4916,7 @@
         <v>8</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L48" s="1">
         <v>7.25</v>
@@ -4946,7 +4946,7 @@
         <v>3.07</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V48" s="2">
         <v>3972</v>
@@ -4967,15 +4967,15 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AB48" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C49" s="1">
         <v>3.47</v>
@@ -4999,7 +4999,7 @@
         <v>3</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L49" s="1">
         <v>7.02</v>
@@ -5050,15 +5050,15 @@
         <v>1</v>
       </c>
       <c r="AB49" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C50" s="1">
         <v>5.24</v>
@@ -5082,7 +5082,7 @@
         <v>3</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L50" s="1">
         <v>3.95</v>
@@ -5112,7 +5112,7 @@
         <v>4.87</v>
       </c>
       <c r="U50" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V50" s="2">
         <v>1698.5</v>
@@ -5133,15 +5133,15 @@
         <v>1</v>
       </c>
       <c r="AB50" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C51" s="1">
         <v>2.2400000000000002</v>
@@ -5165,7 +5165,7 @@
         <v>4</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L51" s="1">
         <v>5.38</v>
@@ -5216,15 +5216,15 @@
         <v>1</v>
       </c>
       <c r="AB51" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C52" s="1">
         <v>7.59</v>
@@ -5248,7 +5248,7 @@
         <v>4</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L52" s="1">
         <v>6.41</v>
@@ -5299,15 +5299,15 @@
         <v>1</v>
       </c>
       <c r="AB52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C53" s="1">
         <v>5.24</v>
@@ -5331,7 +5331,7 @@
         <v>7</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L53" s="1">
         <v>3.93</v>
@@ -5361,7 +5361,7 @@
         <v>2.96</v>
       </c>
       <c r="U53" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V53" s="2">
         <v>4078.5</v>
@@ -5382,15 +5382,15 @@
         <v>1</v>
       </c>
       <c r="AB53" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C54" s="1">
         <v>2.76</v>
@@ -5414,7 +5414,7 @@
         <v>6</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L54" s="1">
         <v>5.36</v>
@@ -5465,15 +5465,15 @@
         <v>1</v>
       </c>
       <c r="AB54" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C55" s="1">
         <v>1.95</v>
@@ -5497,7 +5497,7 @@
         <v>4</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L55" s="1">
         <v>5.49</v>
@@ -5548,15 +5548,15 @@
         <v>1</v>
       </c>
       <c r="AB55" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C56" s="1">
         <v>8.1</v>
@@ -5580,7 +5580,7 @@
         <v>4</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L56" s="1">
         <v>6.74</v>
@@ -5631,15 +5631,15 @@
         <v>1</v>
       </c>
       <c r="AB56" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C57" s="1">
         <v>8.6</v>
@@ -5663,7 +5663,7 @@
         <v>3</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L57" s="1">
         <v>7.22</v>
@@ -5714,15 +5714,15 @@
         <v>1</v>
       </c>
       <c r="AB57" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1">
         <v>7.63</v>
@@ -5746,7 +5746,7 @@
         <v>6</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L58" s="1">
         <v>6.27</v>
@@ -5776,7 +5776,7 @@
         <v>3.89</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V58" s="2">
         <v>5954.6</v>
@@ -5797,15 +5797,15 @@
         <v>1</v>
       </c>
       <c r="AB58" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C59" s="1">
         <v>7.98</v>
@@ -5829,7 +5829,7 @@
         <v>7</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L59" s="1">
         <v>5.6</v>
@@ -5880,15 +5880,15 @@
         <v>1</v>
       </c>
       <c r="AB59" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C60" s="1">
         <v>4.93</v>
@@ -5912,7 +5912,7 @@
         <v>6</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L60" s="1">
         <v>5.66</v>
@@ -5963,15 +5963,15 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AB60" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C61" s="1">
         <v>7.12</v>
@@ -5995,7 +5995,7 @@
         <v>4</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L61" s="1">
         <v>6.88</v>
@@ -6025,7 +6025,7 @@
         <v>2.15</v>
       </c>
       <c r="U61" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V61" s="2">
         <v>3923.6669999999999</v>
@@ -6046,15 +6046,15 @@
         <v>1</v>
       </c>
       <c r="AB61" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C62" s="1">
         <v>4.79</v>
@@ -6078,7 +6078,7 @@
         <v>6</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L62" s="1">
         <v>3.61</v>
@@ -6129,18 +6129,18 @@
         <v>1</v>
       </c>
       <c r="AB62" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D63" s="1">
         <v>7.3</v>
@@ -6161,10 +6161,10 @@
         <v>6</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M63" s="1">
         <v>2.62</v>
@@ -6212,15 +6212,15 @@
         <v>1</v>
       </c>
       <c r="AB63" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B64" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C64" s="1">
         <v>2.74</v>
@@ -6244,7 +6244,7 @@
         <v>7</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L64" s="1">
         <v>5.0599999999999996</v>
@@ -6295,18 +6295,18 @@
         <v>1</v>
       </c>
       <c r="AB64" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D65" s="1">
         <v>5.14</v>
@@ -6327,10 +6327,10 @@
         <v>7</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M65" s="1">
         <v>4.3600000000000003</v>
@@ -6378,15 +6378,15 @@
         <v>1</v>
       </c>
       <c r="AB65" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C66" s="1">
         <v>5.67</v>
@@ -6410,7 +6410,7 @@
         <v>8</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L66" s="1">
         <v>4.4000000000000004</v>
@@ -6461,15 +6461,15 @@
         <v>1</v>
       </c>
       <c r="AB66" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C67" s="1">
         <v>1.93</v>
@@ -6493,7 +6493,7 @@
         <v>6</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L67" s="1">
         <v>5.17</v>
@@ -6523,7 +6523,7 @@
         <v>2.04</v>
       </c>
       <c r="U67" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V67" s="2">
         <v>5299.2</v>
@@ -6544,18 +6544,18 @@
         <v>1</v>
       </c>
       <c r="AB67" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D68" s="1">
         <v>2.85</v>
@@ -6576,10 +6576,10 @@
         <v>7</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M68" s="1">
         <v>5.67</v>
@@ -6627,15 +6627,15 @@
         <v>1</v>
       </c>
       <c r="AB68" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C69" s="1">
         <v>2.15</v>
@@ -6659,7 +6659,7 @@
         <v>6</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L69" s="1">
         <v>5.75</v>
@@ -6710,15 +6710,15 @@
         <v>1</v>
       </c>
       <c r="AB69" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C70" s="1">
         <v>8.1300000000000008</v>
@@ -6742,7 +6742,7 @@
         <v>5</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L70" s="1">
         <v>5.32</v>
@@ -6793,18 +6793,18 @@
         <v>1</v>
       </c>
       <c r="AB70" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D71" s="1">
         <v>4.74</v>
@@ -6825,10 +6825,10 @@
         <v>7</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M71" s="1">
         <v>3.39</v>
@@ -6876,15 +6876,15 @@
         <v>1</v>
       </c>
       <c r="AB71" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B72" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C72" s="1">
         <v>7.65</v>
@@ -6908,7 +6908,7 @@
         <v>6</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L72" s="1">
         <v>4.37</v>
@@ -6959,18 +6959,18 @@
         <v>1</v>
       </c>
       <c r="AB72" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D73" s="1">
         <v>5.78</v>
@@ -6991,10 +6991,10 @@
         <v>4</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M73" s="1">
         <v>3.33</v>
@@ -7042,15 +7042,15 @@
         <v>1</v>
       </c>
       <c r="AB73" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C74" s="1">
         <v>5.57</v>
@@ -7074,7 +7074,7 @@
         <v>4</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L74" s="1">
         <v>4.8</v>
@@ -7125,15 +7125,15 @@
         <v>1</v>
       </c>
       <c r="AB74" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C75" s="1">
         <v>5.5</v>
@@ -7157,7 +7157,7 @@
         <v>5</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L75" s="1">
         <v>4.41</v>
@@ -7208,15 +7208,15 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="AB75" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C76" s="1">
         <v>2.13</v>
@@ -7240,7 +7240,7 @@
         <v>4</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L76" s="1">
         <v>6.5</v>
@@ -7291,18 +7291,18 @@
         <v>1</v>
       </c>
       <c r="AB76" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D77" s="1">
         <v>5.16</v>
@@ -7323,10 +7323,10 @@
         <v>7</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M77" s="1">
         <v>4.4400000000000004</v>
@@ -7374,15 +7374,15 @@
         <v>1</v>
       </c>
       <c r="AB77" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B78" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C78" s="1">
         <v>7.72</v>
@@ -7406,7 +7406,7 @@
         <v>5</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L78" s="1">
         <v>2.95</v>
@@ -7457,15 +7457,15 @@
         <v>1</v>
       </c>
       <c r="AB78" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C79" s="1">
         <v>6.79</v>
@@ -7489,7 +7489,7 @@
         <v>3</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L79" s="1">
         <v>5.0999999999999996</v>
@@ -7540,15 +7540,15 @@
         <v>1</v>
       </c>
       <c r="AB79" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B80" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C80" s="1">
         <v>7.92</v>
@@ -7572,7 +7572,7 @@
         <v>6</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L80" s="1">
         <v>2.97</v>
@@ -7623,15 +7623,15 @@
         <v>1</v>
       </c>
       <c r="AB80" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C81" s="1">
         <v>1.98</v>
@@ -7655,7 +7655,7 @@
         <v>6</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L81" s="1">
         <v>6.05</v>
@@ -7706,15 +7706,15 @@
         <v>1</v>
       </c>
       <c r="AB81" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C82" s="1">
         <v>3.38</v>
@@ -7738,7 +7738,7 @@
         <v>8</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L82" s="1">
         <v>6.07</v>
@@ -7789,15 +7789,15 @@
         <v>1</v>
       </c>
       <c r="AB82" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C83" s="1">
         <v>7.7</v>
@@ -7821,7 +7821,7 @@
         <v>6</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L83" s="1">
         <v>6.53</v>
@@ -7872,18 +7872,18 @@
         <v>1</v>
       </c>
       <c r="AB83" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D84" s="1">
         <v>7</v>
@@ -7904,10 +7904,10 @@
         <v>7</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M84" s="1">
         <v>4.78</v>
@@ -7934,7 +7934,7 @@
         <v>3.11</v>
       </c>
       <c r="U84" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V84" s="2">
         <v>3538.8330000000001</v>
@@ -7955,15 +7955,15 @@
         <v>1</v>
       </c>
       <c r="AB84" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C85" s="1">
         <v>7.53</v>
@@ -7987,7 +7987,7 @@
         <v>6</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L85" s="1">
         <v>4.95</v>
@@ -8038,15 +8038,15 @@
         <v>1</v>
       </c>
       <c r="AB85" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B86" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C86" s="1">
         <v>2.96</v>
@@ -8070,7 +8070,7 @@
         <v>4</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L86" s="1">
         <v>6.39</v>
@@ -8121,15 +8121,15 @@
         <v>1</v>
       </c>
       <c r="AB86" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C87" s="1">
         <v>6.75</v>
@@ -8153,7 +8153,7 @@
         <v>6</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L87" s="1">
         <v>5.85</v>
@@ -8183,7 +8183,7 @@
         <v>3.69</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V87" s="2">
         <v>3756</v>
@@ -8204,15 +8204,15 @@
         <v>1</v>
       </c>
       <c r="AB87" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C88" s="1">
         <v>6.3</v>
@@ -8236,7 +8236,7 @@
         <v>5</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L88" s="1">
         <v>5.3</v>
@@ -8287,15 +8287,15 @@
         <v>1</v>
       </c>
       <c r="AB88" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C89" s="1">
         <v>7.26</v>
@@ -8319,7 +8319,7 @@
         <v>7</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L89" s="1">
         <v>5.12</v>
@@ -8370,18 +8370,18 @@
         <v>0.92300000000000004</v>
       </c>
       <c r="AB89" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B90" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D90" s="1">
         <v>4.63</v>
@@ -8402,10 +8402,10 @@
         <v>7</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M90" s="1">
         <v>3.61</v>
@@ -8453,15 +8453,15 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="AB90" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C91" s="1">
         <v>2.8</v>
@@ -8485,7 +8485,7 @@
         <v>3</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L91" s="1">
         <v>5.78</v>
@@ -8536,15 +8536,15 @@
         <v>1</v>
       </c>
       <c r="AB91" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C92" s="1">
         <v>1.84</v>
@@ -8568,7 +8568,7 @@
         <v>5</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L92" s="1">
         <v>6.21</v>
@@ -8619,15 +8619,15 @@
         <v>1</v>
       </c>
       <c r="AB92" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C93" s="1">
         <v>2.68</v>
@@ -8651,7 +8651,7 @@
         <v>5</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L93" s="1">
         <v>5.36</v>
@@ -8702,15 +8702,15 @@
         <v>1</v>
       </c>
       <c r="AB93" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C94" s="1">
         <v>5.2</v>
@@ -8734,7 +8734,7 @@
         <v>5</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L94" s="1">
         <v>5.2</v>
@@ -8785,15 +8785,15 @@
         <v>1</v>
       </c>
       <c r="AB94" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C95" s="1">
         <v>5.79</v>
@@ -8817,7 +8817,7 @@
         <v>7</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L95" s="1">
         <v>5.48</v>
@@ -8868,15 +8868,15 @@
         <v>0.92</v>
       </c>
       <c r="AB95" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C96" s="1">
         <v>5.33</v>
@@ -8900,7 +8900,7 @@
         <v>6</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L96" s="1">
         <v>3.88</v>
@@ -8951,18 +8951,18 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="AB96" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B97" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D97" s="1">
         <v>4.29</v>
@@ -8983,10 +8983,10 @@
         <v>9</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M97" s="1">
         <v>3.62</v>
@@ -9034,15 +9034,15 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="AB97" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B98" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C98" s="1">
         <v>8.2899999999999991</v>
@@ -9066,7 +9066,7 @@
         <v>7</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L98" s="1">
         <v>6.11</v>
@@ -9117,18 +9117,18 @@
         <v>1</v>
       </c>
       <c r="AB98" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B99" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D99" s="1">
         <v>5.71</v>
@@ -9149,10 +9149,10 @@
         <v>3</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M99" s="1">
         <v>3.1</v>
@@ -9200,15 +9200,15 @@
         <v>1</v>
       </c>
       <c r="AB99" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C100" s="1">
         <v>3.17</v>
@@ -9232,7 +9232,7 @@
         <v>3</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L100" s="1">
         <v>3.81</v>
@@ -9283,15 +9283,15 @@
         <v>1</v>
       </c>
       <c r="AB100" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C101" s="1">
         <v>2.75</v>
@@ -9315,7 +9315,7 @@
         <v>6</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L101" s="1">
         <v>7.07</v>
@@ -9345,7 +9345,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V101" s="2">
         <v>6470.8</v>
@@ -9366,15 +9366,15 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AB101" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B102" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C102" s="1">
         <v>8.0500000000000007</v>
@@ -9398,7 +9398,7 @@
         <v>6</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L102" s="1">
         <v>8.02</v>
@@ -9428,7 +9428,7 @@
         <v>2.46</v>
       </c>
       <c r="U102" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V102" s="2">
         <v>3221.2</v>
@@ -9449,15 +9449,15 @@
         <v>1</v>
       </c>
       <c r="AB102" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B103" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C103" s="1">
         <v>3.28</v>
@@ -9481,7 +9481,7 @@
         <v>7</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L103" s="1">
         <v>4.83</v>
@@ -9532,15 +9532,15 @@
         <v>1</v>
       </c>
       <c r="AB103" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="104" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B104" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C104" s="1">
         <v>1.56</v>
@@ -9564,7 +9564,7 @@
         <v>7</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L104" s="1">
         <v>6.1</v>
@@ -9615,15 +9615,15 @@
         <v>1</v>
       </c>
       <c r="AB104" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B105" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C105" s="1">
         <v>5.4</v>
@@ -9647,7 +9647,7 @@
         <v>5</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L105" s="1">
         <v>5.03</v>
@@ -9698,15 +9698,15 @@
         <v>1</v>
       </c>
       <c r="AB105" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B106" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C106" s="1">
         <v>3.03</v>
@@ -9730,7 +9730,7 @@
         <v>7</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L106" s="1">
         <v>6.85</v>
@@ -9781,15 +9781,15 @@
         <v>1</v>
       </c>
       <c r="AB106" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B107" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C107" s="1">
         <v>6.48</v>
@@ -9813,7 +9813,7 @@
         <v>5</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L107" s="1">
         <v>4.79</v>
@@ -9864,18 +9864,18 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="AB107" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B108" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D108" s="1">
         <v>4.8099999999999996</v>
@@ -9896,10 +9896,10 @@
         <v>4</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M108" s="1">
         <v>3.86</v>
@@ -9947,15 +9947,15 @@
         <v>1</v>
       </c>
       <c r="AB108" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B109" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C109" s="1">
         <v>8.32</v>
@@ -9979,7 +9979,7 @@
         <v>7</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L109" s="1">
         <v>6.63</v>
@@ -10009,7 +10009,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V109" s="2">
         <v>2802.1669999999999</v>
@@ -10030,15 +10030,15 @@
         <v>1</v>
       </c>
       <c r="AB109" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B110" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C110" s="1">
         <v>4.84</v>
@@ -10062,7 +10062,7 @@
         <v>7</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L110" s="1">
         <v>6.33</v>
@@ -10092,7 +10092,7 @@
         <v>4.75</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V110" s="2">
         <v>2717.8330000000001</v>
@@ -10113,18 +10113,18 @@
         <v>1</v>
       </c>
       <c r="AB110" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D111" s="1">
         <v>6</v>
@@ -10145,10 +10145,10 @@
         <v>4</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M111" s="1">
         <v>3.43</v>
@@ -10196,18 +10196,18 @@
         <v>1</v>
       </c>
       <c r="AB111" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D112" s="1">
         <v>5.79</v>
@@ -10228,10 +10228,10 @@
         <v>5</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M112" s="1">
         <v>3.58</v>
@@ -10279,15 +10279,15 @@
         <v>1</v>
       </c>
       <c r="AB112" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B113" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C113" s="1">
         <v>3.97</v>
@@ -10311,7 +10311,7 @@
         <v>6</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L113" s="1">
         <v>6.03</v>
@@ -10362,15 +10362,15 @@
         <v>1</v>
       </c>
       <c r="AB113" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B114" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C114" s="1">
         <v>8.3800000000000008</v>
@@ -10394,7 +10394,7 @@
         <v>3</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L114" s="1">
         <v>7.72</v>
@@ -10445,15 +10445,15 @@
         <v>1</v>
       </c>
       <c r="AB114" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B115" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C115" s="1">
         <v>5.79</v>
@@ -10477,7 +10477,7 @@
         <v>6</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L115" s="1">
         <v>5.32</v>
@@ -10528,7 +10528,7 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AB115" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>